<commit_message>
pointing correct file, data_prep.ipynb
</commit_message>
<xml_diff>
--- a/1DConv.xlsx
+++ b/1DConv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\1DCNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4587FD5A-4B42-457F-A4D8-04E40CEF1BA2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F9F753-64D0-4789-A93F-D428C4A923CB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12132" windowHeight="4908" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6987,15 +6987,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>176893</xdr:colOff>
+      <xdr:colOff>149999</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9523</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>354106</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>13606</xdr:rowOff>
+      <xdr:rowOff>4083</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7523,8 +7523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2049"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7587,7 +7587,7 @@
         <v>5.9941363636363799E-2</v>
       </c>
       <c r="J2" s="1">
-        <f t="shared" ref="J2:L2" si="0">SUMPRODUCT($A2:$A17,D$2:D$17)</f>
+        <f>SUMPRODUCT($A2:$A17,D$2:D$17)</f>
         <v>-6.7697272727272786E-2</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -7619,14 +7619,14 @@
         <v>6.2684181818182028E-2</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J55" si="1">SUMPRODUCT($A3:$A18,D$2:D$17)</f>
+        <f t="shared" ref="J3:J55" si="0">SUMPRODUCT($A3:$A18,D$2:D$17)</f>
         <v>-6.3321090909091091E-2</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L55" si="2">SUMPRODUCT($A3:$A18,F$2:F$17)</f>
+        <f t="shared" ref="L3:L55" si="1">SUMPRODUCT($A3:$A18,F$2:F$17)</f>
         <v>-3.6077818181817843E-2</v>
       </c>
     </row>
@@ -7651,14 +7651,14 @@
         <v>3.5297090909091167E-2</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-3.4875909090909374E-2</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.4381818181816554E-3</v>
       </c>
     </row>
@@ -7679,18 +7679,18 @@
         <v>0.2</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I54" si="3">SUMPRODUCT($A5:$A20,C$2:C$17)</f>
+        <f t="shared" ref="I5:I54" si="2">SUMPRODUCT($A5:$A20,C$2:C$17)</f>
         <v>1.498790909090927E-2</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-1.8162181818182029E-2</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-2.6791272727272671E-2</v>
       </c>
     </row>
@@ -7711,18 +7711,18 @@
         <v>0.4</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6.9854545454547633E-3</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-2.2702727272730511E-3</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.4098181818180644E-3</v>
       </c>
     </row>
@@ -7743,18 +7743,18 @@
         <v>0.2</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-2.1644636363636109E-2</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.5096272727272464E-2</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.6940727272726945E-2</v>
       </c>
     </row>
@@ -7775,18 +7775,18 @@
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.8542272727272786E-2</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-2.1798727272727227E-2</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-2.8188363636363623E-2</v>
       </c>
     </row>
@@ -7807,18 +7807,18 @@
         <v>-0.2</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-2.2497272727272637E-2</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.2456181818181799E-2</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.8408727272727285E-2</v>
       </c>
     </row>
@@ -7839,18 +7839,18 @@
         <v>-0.4</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-7.5216909090908946E-2</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.8539636363636455E-2</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.8618181818179926E-4</v>
       </c>
     </row>
@@ -7871,18 +7871,18 @@
         <v>-0.2</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-9.3522909090909018E-2</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.129836363636378E-2</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.8326545454545481E-2</v>
       </c>
     </row>
@@ -7903,18 +7903,18 @@
         <v>0</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.12280018181818174</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.11350336363636375</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.072109090909086E-2</v>
       </c>
     </row>
@@ -7935,18 +7935,18 @@
         <v>0.2</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.19593172727272706</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.17158536363636398</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.3489090909090823E-2</v>
       </c>
     </row>
@@ -7967,18 +7967,18 @@
         <v>0.4</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.24135772727272684</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.200359272727273</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-3.492727272727264E-2</v>
       </c>
     </row>
@@ -7999,18 +7999,18 @@
         <v>0.2</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.24021745454545415</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.19846909090909118</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.210327272727272E-2</v>
       </c>
     </row>
@@ -8031,18 +8031,18 @@
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.23898472727272702</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.19591118181818215</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.14098290909090896</v>
       </c>
     </row>
@@ -8063,18 +8063,18 @@
         <v>-0.2</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.18580281818181793</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1386715454545456</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8.6496363636363482E-2</v>
       </c>
     </row>
@@ -8086,18 +8086,18 @@
         <v>10</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.20334863636363595</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.14922163636363639</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.8244363636363614E-2</v>
       </c>
     </row>
@@ -8109,18 +8109,18 @@
         <v>6</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.14700272727272698</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.6660727272727389E-2</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-5.013090909090908E-2</v>
       </c>
     </row>
@@ -8132,18 +8132,18 @@
         <v>7</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-8.0825818181817971E-2</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.3658090909091045E-2</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-6.7841090909090893E-2</v>
       </c>
     </row>
@@ -8152,18 +8152,18 @@
         <v>-6.4923636363636295E-2</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-9.0882818181817815E-2</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.1393454545454572E-2</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.4957090909090785E-2</v>
       </c>
     </row>
@@ -8172,18 +8172,18 @@
         <v>4.2529090909090898E-2</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-4.8240727272726887E-2</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-1.9846909090909033E-2</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.561454545454541E-2</v>
       </c>
     </row>
@@ -8192,18 +8192,18 @@
         <v>1.2532727272727201E-2</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-6.6156363636360131E-3</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-6.0526909090908916E-2</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.7803636363636241E-2</v>
       </c>
     </row>
@@ -8212,18 +8212,18 @@
         <v>2.3216363636363601E-2</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.0340000000000337E-2</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-9.1252636363636008E-2</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.10572690909090876</v>
       </c>
     </row>
@@ -8232,11 +8232,11 @@
         <v>0.132312727272727</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4.3094090909091082E-2</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.11770490909090858</v>
       </c>
       <c r="K25" s="1" t="s">
@@ -8252,18 +8252,18 @@
         <v>8.6701818181818102E-2</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8.0805272727272975E-2</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.14679727272727239</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.7609454545454429E-2</v>
       </c>
     </row>
@@ -8272,18 +8272,18 @@
         <v>2.2599999999999901E-2</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.3902000000000356E-2</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.1403357272727267</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.3829090909092228E-3</v>
       </c>
     </row>
@@ -8292,18 +8292,18 @@
         <v>0.25353090909090897</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.11888627272727308</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.18574118181818133</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.11230145454545418</v>
       </c>
     </row>
@@ -8312,18 +8312,18 @@
         <v>0.25373636363636298</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.12344736363636369</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.17273590909090866</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-6.2088363636363303E-2</v>
       </c>
     </row>
@@ -8332,18 +8332,18 @@
         <v>5.7321818181818099E-2</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6.3434090909090912E-2</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.10101172727272699</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-5.5472727272727184E-3</v>
       </c>
     </row>
@@ -8352,18 +8352,18 @@
         <v>6.3896363636363598E-2</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.11424300000000001</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.14443454545454529</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-4.2734545454545581E-2</v>
       </c>
     </row>
@@ -8372,18 +8372,18 @@
         <v>2.7941818181818099E-2</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.15470727272727264</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.17722509090909078</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-4.4378181818182032E-2</v>
       </c>
     </row>
@@ -8392,18 +8392,18 @@
         <v>0.150803636363636</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.16087090909090895</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.18263881818181796</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-5.8143636363636425E-2</v>
       </c>
     </row>
@@ -8412,18 +8412,18 @@
         <v>5.9376363636363602E-2</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.16809263636363594</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.17659845454545428</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-3.1188000000000167E-2</v>
       </c>
     </row>
@@ -8432,18 +8432,18 @@
         <v>-3.9036363636363598E-2</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.1848988181818178</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.18642945454545423</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.2458181818183071E-3</v>
       </c>
     </row>
@@ -8452,18 +8452,18 @@
         <v>0.107247272727272</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.18355309090909055</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.18934690909090865</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-3.1722181818181344E-2</v>
       </c>
     </row>
@@ -8472,18 +8472,18 @@
         <v>0.107041818181818</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.16271999999999995</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.16111745454545445</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-4.6268363636363233E-2</v>
       </c>
     </row>
@@ -8492,18 +8492,18 @@
         <v>2.3627272727272702E-2</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.709781818181823E-2</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-9.2793545454545337E-2</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.2461818181819639E-3</v>
       </c>
     </row>
@@ -8512,18 +8512,18 @@
         <v>8.7934545454545404E-2</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.0963000000000022E-2</v>
       </c>
       <c r="J39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-4.9524818181817976E-2</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.3190181818181834E-2</v>
       </c>
     </row>
@@ -8532,18 +8532,18 @@
         <v>9.7180000000000002E-2</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.6211363636363687E-2</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-2.7643909090908993E-2</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-9.738545454545635E-3</v>
       </c>
     </row>
@@ -8552,18 +8552,18 @@
         <v>-4.0063636363636301E-2</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-2.371972727272724E-2</v>
       </c>
       <c r="J41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.5584727272727393E-2</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.9309090909090587E-2</v>
       </c>
     </row>
@@ -8572,18 +8572,18 @@
         <v>9.55363636363636E-2</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-5.1610181818181812E-2</v>
       </c>
       <c r="J42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.7465636363636476E-2</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-3.2872727272727373E-2</v>
       </c>
     </row>
@@ -8592,18 +8592,18 @@
         <v>3.1023636363636298E-2</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.10324090909090905</v>
       </c>
       <c r="J43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.11292809090909089</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-4.1707272727272662E-2</v>
       </c>
     </row>
@@ -8612,18 +8612,18 @@
         <v>-9.7796363636363598E-2</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.14111645454545457</v>
       </c>
       <c r="J44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.15038245454545454</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.7116363636365193E-3</v>
       </c>
     </row>
@@ -8632,18 +8632,18 @@
         <v>1.9518181818181799E-2</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.15293009090909071</v>
       </c>
       <c r="J45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.15209799999999987</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-5.6951999999999586E-2</v>
       </c>
     </row>
@@ -8652,18 +8652,18 @@
         <v>-9.0399999999999897E-2</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.18431327272727246</v>
       </c>
       <c r="J46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.18140609090909068</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-4.396727272727172E-3</v>
       </c>
     </row>
@@ -8672,18 +8672,18 @@
         <v>-8.9578181818181807E-2</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.20556754545454511</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.19060018181818161</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.7228363636363546E-2</v>
       </c>
     </row>
@@ -8692,18 +8692,18 @@
         <v>1.29436363636363E-2</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.20646127272727233</v>
       </c>
       <c r="J48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.18055345454545443</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.9611636363635981E-2</v>
       </c>
     </row>
@@ -8712,18 +8712,18 @@
         <v>-0.114438181818181</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.1798138181818178</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.15529281818181795</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.12734072727272672</v>
       </c>
     </row>
@@ -8732,18 +8732,18 @@
         <v>-8.01272727272727E-2</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.12767972727272714</v>
       </c>
       <c r="J50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.5166545454545615E-2</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.11267127272727259</v>
       </c>
     </row>
@@ -8752,18 +8752,18 @@
         <v>4.62272727272727E-2</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-8.3743272727272514E-2</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.4645272727272839E-2</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.8408727272727365E-2</v>
       </c>
     </row>
@@ -8772,18 +8772,18 @@
         <v>-4.0680000000000001E-2</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-6.3711454545454349E-2</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.6852909090909129E-2</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-9.7796363636360982E-3</v>
       </c>
     </row>
@@ -8792,18 +8792,18 @@
         <v>5.3007272727272702E-2</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-4.8281818181817255E-3</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-3.3345272727272599E-2</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-4.2323636363636168E-2</v>
       </c>
     </row>
@@ -8812,18 +8812,18 @@
         <v>8.0949090909090901E-2</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-3.965272727272701E-3</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-3.3571272727272596E-2</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-6.6402909090908971E-2</v>
       </c>
     </row>
@@ -8836,14 +8836,14 @@
         <v>-4.5200000000001055E-4</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-3.3242545454545296E-2</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.5696727272727341E-2</v>
       </c>
     </row>
@@ -18868,7 +18868,7 @@
   <dimension ref="A1:T2049"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44437,6 +44437,77 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="f2fcef57-0513-4f79-abb5-87f72d6fd615">MMFZ2WNJ7E4J-300305979-5</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="f2fcef57-0513-4f79-abb5-87f72d6fd615">
+      <Url>http://edc.micron.com/imft/OE001/_layouts/15/DocIdRedir.aspx?ID=MMFZ2WNJ7E4J-300305979-5</Url>
+      <Description>MMFZ2WNJ7E4J-300305979-5</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039D7EE82107D914389F38517A34C5E0B" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bd430a0082727580b82253c1b736c36">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f2fcef57-0513-4f79-abb5-87f72d6fd615" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd4ab6e925caf70b9b9be9a92596203c" ns2:_="">
     <xsd:import namespace="f2fcef57-0513-4f79-abb5-87f72d6fd615"/>
@@ -44601,78 +44672,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6038490A-3359-4156-9201-DD4BAC84580D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f2fcef57-0513-4f79-abb5-87f72d6fd615"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C0CA0AB-50FB-43CA-8082-14D30762A6F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="f2fcef57-0513-4f79-abb5-87f72d6fd615">MMFZ2WNJ7E4J-300305979-5</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="f2fcef57-0513-4f79-abb5-87f72d6fd615">
-      <Url>http://edc.micron.com/imft/OE001/_layouts/15/DocIdRedir.aspx?ID=MMFZ2WNJ7E4J-300305979-5</Url>
-      <Description>MMFZ2WNJ7E4J-300305979-5</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BF304C-684E-44B9-899D-1C93F735CCDE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4C252D2-B715-4190-8324-B89D93730D16}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44688,36 +44720,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BF304C-684E-44B9-899D-1C93F735CCDE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C0CA0AB-50FB-43CA-8082-14D30762A6F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6038490A-3359-4156-9201-DD4BAC84580D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f2fcef57-0513-4f79-abb5-87f72d6fd615"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>